<commit_message>
ADD /branches/Kim/Report/Kim's report 01_02_2011.xlsx
</commit_message>
<xml_diff>
--- a/Report/Kim's report 30_01_2011.xlsx
+++ b/Report/Kim's report 30_01_2011.xlsx
@@ -63,10 +63,10 @@
     <t>Có một lỗi trong file KB, 2 phần trong implication giống nhau</t>
   </si>
   <si>
-    <t>29/01/2011-30/01/2011</t>
-  </si>
-  <si>
     <t>Code chương trình nhâp parse file IDMEF</t>
+  </si>
+  <si>
+    <t>31/01/2011-01/02/2011</t>
   </si>
 </sst>
 </file>
@@ -152,14 +152,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -466,7 +466,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -475,24 +475,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:19">
       <c r="D3" s="1"/>
@@ -524,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -579,12 +579,12 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>1</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="5" t="s">
         <v>14</v>
       </c>
@@ -597,18 +597,18 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>0.1</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
@@ -631,13 +631,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="O7:S7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K8:N8"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D1:J2"/>
     <mergeCell ref="B7:F7"/>
@@ -646,6 +639,13 @@
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="O7:S7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K8:N8"/>
     <mergeCell ref="K7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>